<commit_message>
Tablas basales con arreglos en la parte del orden y añadiendo el conteo de NA's para todo, sin estratificar.
</commit_message>
<xml_diff>
--- a/Outputs/Tablas_basales/Tabla_basal_con_missings.xlsx
+++ b/Outputs/Tablas_basales/Tabla_basal_con_missings.xlsx
@@ -464,6 +464,11 @@
           <t>IMC (missing values)</t>
         </is>
       </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
       <c r="D4" t="inlineStr">
         <is>
           <t>2</t>
@@ -518,6 +523,11 @@
           <t>Pes (missing values)</t>
         </is>
       </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="D6" t="inlineStr">
         <is>
           <t>1</t>
@@ -572,6 +582,11 @@
           <t>Talla_m (missing values)</t>
         </is>
       </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
       <c r="D8" t="inlineStr">
         <is>
           <t>2</t>
@@ -626,6 +641,11 @@
           <t>edat_IQ (missing values)</t>
         </is>
       </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
       <c r="D10" t="inlineStr">
         <is>
           <t>0</t>
@@ -739,6 +759,11 @@
           <t>ALT_preIQ (missing values)</t>
         </is>
       </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
       <c r="D14" t="inlineStr">
         <is>
           <t>1</t>
@@ -793,6 +818,11 @@
           <t>AST_preIQ (missing values)</t>
         </is>
       </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
       <c r="D16" t="inlineStr">
         <is>
           <t>1</t>
@@ -847,6 +877,11 @@
           <t>Alb_gL_preIQ (missing values)</t>
         </is>
       </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
       <c r="D18" t="inlineStr">
         <is>
           <t>1</t>
@@ -901,6 +936,11 @@
           <t>BB_mgdL_preIQ (missing values)</t>
         </is>
       </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="D20" t="inlineStr">
         <is>
           <t>1</t>
@@ -955,6 +995,11 @@
           <t>Creat_mgdL_preIQ (missing values)</t>
         </is>
       </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="D22" t="inlineStr">
         <is>
           <t>1</t>
@@ -1009,6 +1054,11 @@
           <t>FA_preIQ (missing values)</t>
         </is>
       </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>204</t>
+        </is>
+      </c>
       <c r="D24" t="inlineStr">
         <is>
           <t>194</t>
@@ -1063,6 +1113,11 @@
           <t>FsC_Elastografia (missing values)</t>
         </is>
       </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>189</t>
+        </is>
+      </c>
       <c r="D26" t="inlineStr">
         <is>
           <t>90</t>
@@ -1117,6 +1172,11 @@
           <t>GGT_preIQ (missing values)</t>
         </is>
       </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>204</t>
+        </is>
+      </c>
       <c r="D28" t="inlineStr">
         <is>
           <t>194</t>
@@ -1171,6 +1231,11 @@
           <t>HVPG_basal (missing values)</t>
         </is>
       </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>121</t>
+        </is>
+      </c>
       <c r="D30" t="inlineStr">
         <is>
           <t>0</t>
@@ -1225,6 +1290,11 @@
           <t>INR_preIQ (missing values)</t>
         </is>
       </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="D32" t="inlineStr">
         <is>
           <t>1</t>
@@ -1279,6 +1349,11 @@
           <t>K_preIQ (missing values)</t>
         </is>
       </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>195</t>
+        </is>
+      </c>
       <c r="D34" t="inlineStr">
         <is>
           <t>194</t>
@@ -1333,6 +1408,11 @@
           <t>Leucos_preIQ (missing values)</t>
         </is>
       </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>194</t>
+        </is>
+      </c>
       <c r="D36" t="inlineStr">
         <is>
           <t>194</t>
@@ -1387,6 +1467,11 @@
           <t>MELD_1anyspostIQ (missing values)</t>
         </is>
       </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>221</t>
+        </is>
+      </c>
       <c r="D38" t="inlineStr">
         <is>
           <t>194</t>
@@ -1441,6 +1526,11 @@
           <t>MELD_basal (missing values)</t>
         </is>
       </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
       <c r="D40" t="inlineStr">
         <is>
           <t>3</t>
@@ -1495,6 +1585,11 @@
           <t>NA_preIQ_ (missing values)</t>
         </is>
       </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>194</t>
+        </is>
+      </c>
       <c r="D42" t="inlineStr">
         <is>
           <t>194</t>
@@ -1549,6 +1644,11 @@
           <t>PCR_preIQ (missing values)</t>
         </is>
       </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>304</t>
+        </is>
+      </c>
       <c r="D44" t="inlineStr">
         <is>
           <t>194</t>
@@ -1603,6 +1703,11 @@
           <t>Pughpunts_basal (missing values)</t>
         </is>
       </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="D46" t="inlineStr">
         <is>
           <t>1</t>
@@ -1657,6 +1762,11 @@
           <t>Urea_mgdL_preIQ (missing values)</t>
         </is>
       </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="D48" t="inlineStr">
         <is>
           <t>1</t>
@@ -1711,6 +1821,11 @@
           <t>plaquetes_preIQ (missing values)</t>
         </is>
       </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="D50" t="inlineStr">
         <is>
           <t>2</t>
@@ -1723,6 +1838,11 @@
       </c>
     </row>
     <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>DIabetes (%)</t>
+        </is>
+      </c>
       <c r="B51" t="inlineStr">
         <is>
           <t>insulina</t>
@@ -1745,11 +1865,6 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>DIabetes (%)</t>
-        </is>
-      </c>
       <c r="B52" t="inlineStr">
         <is>
           <t>no</t>
@@ -2145,6 +2260,11 @@
       </c>
     </row>
     <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>HTA (%)</t>
+        </is>
+      </c>
       <c r="B67" t="inlineStr">
         <is>
           <t>IECA</t>
@@ -2167,11 +2287,6 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>HTA (%)</t>
-        </is>
-      </c>
       <c r="B68" t="inlineStr">
         <is>
           <t>ninguno</t>
@@ -2699,6 +2814,11 @@
       </c>
     </row>
     <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>dislipemias (%)</t>
+        </is>
+      </c>
       <c r="B89" t="inlineStr">
         <is>
           <t>No</t>
@@ -2721,11 +2841,6 @@
       </c>
     </row>
     <row r="90">
-      <c r="A90" t="inlineStr">
-        <is>
-          <t>dislipemias (%)</t>
-        </is>
-      </c>
       <c r="B90" t="inlineStr">
         <is>
           <t>Si</t>
@@ -2758,6 +2873,11 @@
       </c>
     </row>
     <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>etiologiaCH (%)</t>
+        </is>
+      </c>
       <c r="B91" t="inlineStr">
         <is>
           <t>Altres</t>
@@ -2824,11 +2944,6 @@
       </c>
     </row>
     <row r="94">
-      <c r="A94" t="inlineStr">
-        <is>
-          <t>etiologiaCH (%)</t>
-        </is>
-      </c>
       <c r="B94" t="inlineStr">
         <is>
           <t>OH</t>

</xml_diff>

<commit_message>
Propensity scores en fase de creación
</commit_message>
<xml_diff>
--- a/Outputs/Tablas_basales/Tabla_basal_con_missings.xlsx
+++ b/Outputs/Tablas_basales/Tabla_basal_con_missings.xlsx
@@ -412,7 +412,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t xml:space="preserve">  194</t>
+          <t xml:space="preserve">   194</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -434,7 +434,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>27.07 [24.22, 30.21]</t>
+          <t xml:space="preserve"> 27.07 [24.22, 30.21]</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -493,7 +493,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>73.00 [68.00, 83.00]</t>
+          <t xml:space="preserve"> 73.00 [68.00, 83.00]</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -552,7 +552,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 1.67 [1.59, 1.73]</t>
+          <t xml:space="preserve">  1.67 [1.59, 1.73]</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -611,7 +611,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>65.00 [55.00, 71.75]</t>
+          <t xml:space="preserve"> 65.00 [55.00, 71.75]</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -675,7 +675,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t xml:space="preserve">   72 ( 37.1) </t>
+          <t xml:space="preserve">    72 ( 37.1) </t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -707,7 +707,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t xml:space="preserve">  122 ( 62.9) </t>
+          <t xml:space="preserve">   122 ( 62.9) </t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -729,7 +729,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>44.00 [28.00, 78.00]</t>
+          <t xml:space="preserve"> 44.00 [28.00, 78.00]</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -788,7 +788,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>58.00 [37.00, 88.00]</t>
+          <t xml:space="preserve"> 58.00 [37.00, 88.00]</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>37.00 [34.00, 40.70]</t>
+          <t xml:space="preserve"> 37.00 [34.00, 40.70]</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -906,7 +906,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 1.17 [0.82, 1.58]</t>
+          <t xml:space="preserve">  1.17 [0.82, 1.58]</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -965,7 +965,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.80 [0.70, 0.93]</t>
+          <t xml:space="preserve">  0.80 [0.70, 0.93]</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1019,22 +1019,22 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
+          <t xml:space="preserve"> 98.00 [76.00, 139.00]</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>101.00 [79.00, 148.75]</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
           <t xml:space="preserve"> 91.00 [72.00, 127.00]</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   NA [NA, NA]</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 91.00 [72.00, 127.00]</t>
-        </is>
-      </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t xml:space="preserve">    NA</t>
+          <t xml:space="preserve"> 0.020</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -1044,7 +1044,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t xml:space="preserve">    NA</t>
+          <t xml:space="preserve"> 0.070</t>
         </is>
       </c>
     </row>
@@ -1056,12 +1056,12 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>204</t>
+          <t>46</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>194</t>
+          <t>36</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1083,7 +1083,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>28.50 [18.90, 39.60]</t>
+          <t xml:space="preserve"> 28.50 [18.90, 39.60]</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1137,22 +1137,22 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
+          <t xml:space="preserve"> 75.50 [41.00, 130.50]</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 74.00 [47.00, 113.00]</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
           <t xml:space="preserve"> 77.00 [37.50, 140.00]</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   NA [NA, NA]</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 77.00 [37.50, 140.00]</t>
-        </is>
-      </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t xml:space="preserve">    NA</t>
+          <t xml:space="preserve"> 0.467</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
@@ -1162,7 +1162,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t xml:space="preserve">    NA</t>
+          <t xml:space="preserve"> 0.246</t>
         </is>
       </c>
     </row>
@@ -1174,12 +1174,12 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>204</t>
+          <t>47</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>194</t>
+          <t>37</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -1201,7 +1201,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>17.00 [14.00, 20.50]</t>
+          <t xml:space="preserve"> 17.00 [14.00, 20.50]</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -1260,7 +1260,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 1.16 [1.09, 1.26]</t>
+          <t xml:space="preserve">  1.16 [1.09, 1.26]</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -1314,22 +1314,22 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
+          <t xml:space="preserve">  4.10 [4.00, 4.42]</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  4.00 [4.00, 4.20]</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
           <t xml:space="preserve">  4.29 [3.93, 4.57]</t>
         </is>
       </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   NA [NA, NA]</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  4.29 [3.93, 4.57]</t>
-        </is>
-      </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t xml:space="preserve">    NA</t>
+          <t>&lt;0.001</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
@@ -1339,7 +1339,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t xml:space="preserve">    NA</t>
+          <t xml:space="preserve"> 0.305</t>
         </is>
       </c>
     </row>
@@ -1351,12 +1351,12 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>195</t>
+          <t>39</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>194</t>
+          <t>38</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -1378,7 +1378,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t xml:space="preserve">   NA [NA, NA]</t>
+          <t xml:space="preserve">    NA [NA, NA]</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -1437,7 +1437,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t xml:space="preserve">   NA [NA, NA]</t>
+          <t xml:space="preserve">    NA [NA, NA]</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -1496,7 +1496,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 9.04 [7.91, 10.45]</t>
+          <t xml:space="preserve">  9.04 [7.91, 10.45]</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -1550,22 +1550,22 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
+          <t>140.00 [138.00, 142.00]</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>141.00 [139.00, 142.00]</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
           <t>139.00 [138.00, 141.00]</t>
         </is>
       </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   NA [NA, NA]</t>
-        </is>
-      </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>139.00 [138.00, 141.00]</t>
-        </is>
-      </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t xml:space="preserve">    NA</t>
+          <t>&lt;0.001</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
@@ -1575,7 +1575,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t xml:space="preserve">    NA</t>
+          <t xml:space="preserve"> 0.388</t>
         </is>
       </c>
     </row>
@@ -1587,12 +1587,12 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>194</t>
+          <t>39</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>194</t>
+          <t>39</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -1614,7 +1614,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t xml:space="preserve">   NA [NA, NA]</t>
+          <t xml:space="preserve">    NA [NA, NA]</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -1673,7 +1673,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 5.00 [5.00, 6.00]</t>
+          <t xml:space="preserve">  5.00 [5.00, 6.00]</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
@@ -1732,7 +1732,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 5.00 [4.00, 6.30]</t>
+          <t xml:space="preserve">  5.00 [4.00, 6.30]</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -1791,7 +1791,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>95.00 [70.75, 123.00]</t>
+          <t xml:space="preserve"> 95.00 [70.75, 123.00]</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
@@ -1855,7 +1855,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t xml:space="preserve">   67 ( 34.5) </t>
+          <t xml:space="preserve">    67 ( 34.5) </t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
@@ -1877,7 +1877,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t xml:space="preserve">  126 ( 64.9) </t>
+          <t xml:space="preserve">   126 ( 64.9) </t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
@@ -1904,7 +1904,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t xml:space="preserve">    1 (  0.5) </t>
+          <t xml:space="preserve">     1 (  0.5) </t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
@@ -1931,7 +1931,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t xml:space="preserve">  158 ( 81.4) </t>
+          <t xml:space="preserve">   158 ( 81.4) </t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
@@ -1963,7 +1963,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t xml:space="preserve">   36 ( 18.6) </t>
+          <t xml:space="preserve">    36 ( 18.6) </t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
@@ -1990,7 +1990,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t xml:space="preserve">    1 (  0.5) </t>
+          <t xml:space="preserve">     1 (  0.5) </t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
@@ -2022,7 +2022,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t xml:space="preserve">  103 ( 53.1) </t>
+          <t xml:space="preserve">   103 ( 53.1) </t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
@@ -2039,7 +2039,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t xml:space="preserve">   90 ( 46.4) </t>
+          <t xml:space="preserve">    90 ( 46.4) </t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
@@ -2066,7 +2066,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t xml:space="preserve">   17 (  8.8) </t>
+          <t xml:space="preserve">    17 (  8.8) </t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
@@ -2098,7 +2098,7 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t xml:space="preserve">   87 ( 44.8) </t>
+          <t xml:space="preserve">    87 ( 44.8) </t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
@@ -2115,7 +2115,7 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t xml:space="preserve">   90 ( 46.4) </t>
+          <t xml:space="preserve">    90 ( 46.4) </t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
@@ -2142,7 +2142,7 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t xml:space="preserve">   43 ( 22.2) </t>
+          <t xml:space="preserve">    43 ( 22.2) </t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
@@ -2174,7 +2174,7 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t xml:space="preserve">   61 ( 31.4) </t>
+          <t xml:space="preserve">    61 ( 31.4) </t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
@@ -2191,7 +2191,7 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t xml:space="preserve">   90 ( 46.4) </t>
+          <t xml:space="preserve">    90 ( 46.4) </t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
@@ -2218,7 +2218,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t xml:space="preserve">  188 ( 96.9) </t>
+          <t xml:space="preserve">   188 ( 96.9) </t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
@@ -2250,7 +2250,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t xml:space="preserve">    6 (  3.1) </t>
+          <t xml:space="preserve">     6 (  3.1) </t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
@@ -2277,7 +2277,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t xml:space="preserve">   86 ( 44.3) </t>
+          <t xml:space="preserve">    86 ( 44.3) </t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
@@ -2299,7 +2299,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t xml:space="preserve">  105 ( 54.1) </t>
+          <t xml:space="preserve">   105 ( 54.1) </t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
@@ -2326,7 +2326,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t xml:space="preserve">    3 (  1.5) </t>
+          <t xml:space="preserve">     3 (  1.5) </t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
@@ -2353,7 +2353,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t xml:space="preserve">    0 (  0.0) </t>
+          <t xml:space="preserve">     0 (  0.0) </t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
@@ -2385,7 +2385,7 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t xml:space="preserve">  194 (100.0) </t>
+          <t xml:space="preserve">   194 (100.0) </t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
@@ -2402,7 +2402,7 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t xml:space="preserve">    0 (  0.0) </t>
+          <t xml:space="preserve">     0 (  0.0) </t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
@@ -2429,7 +2429,7 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t xml:space="preserve">   70 ( 36.1) </t>
+          <t xml:space="preserve">    70 ( 36.1) </t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
@@ -2461,7 +2461,7 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t xml:space="preserve">  124 ( 63.9) </t>
+          <t xml:space="preserve">   124 ( 63.9) </t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
@@ -2478,7 +2478,7 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t xml:space="preserve">    0 (  0.0) </t>
+          <t xml:space="preserve">     0 (  0.0) </t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
@@ -2505,7 +2505,7 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t xml:space="preserve">  136 ( 70.1) </t>
+          <t xml:space="preserve">   136 ( 70.1) </t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
@@ -2537,7 +2537,7 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t xml:space="preserve">   58 ( 29.9) </t>
+          <t xml:space="preserve">    58 ( 29.9) </t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
@@ -2554,7 +2554,7 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t xml:space="preserve">    0 (  0.0) </t>
+          <t xml:space="preserve">     0 (  0.0) </t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
@@ -2581,7 +2581,7 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t xml:space="preserve">  166 ( 85.6) </t>
+          <t xml:space="preserve">   166 ( 85.6) </t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
@@ -2613,7 +2613,7 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t xml:space="preserve">   27 ( 13.9) </t>
+          <t xml:space="preserve">    27 ( 13.9) </t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
@@ -2635,7 +2635,7 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t xml:space="preserve">    0 (  0.0) </t>
+          <t xml:space="preserve">     0 (  0.0) </t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
@@ -2652,7 +2652,7 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t xml:space="preserve">    1 (  0.5) </t>
+          <t xml:space="preserve">     1 (  0.5) </t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
@@ -2679,7 +2679,7 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t xml:space="preserve">    3 (  1.5) </t>
+          <t xml:space="preserve">     3 (  1.5) </t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
@@ -2711,7 +2711,7 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t xml:space="preserve">  191 ( 98.5) </t>
+          <t xml:space="preserve">   191 ( 98.5) </t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
@@ -2728,7 +2728,7 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t xml:space="preserve">    0 (  0.0) </t>
+          <t xml:space="preserve">     0 (  0.0) </t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
@@ -2755,7 +2755,7 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t xml:space="preserve">  173 ( 89.2) </t>
+          <t xml:space="preserve">   173 ( 89.2) </t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
@@ -2787,7 +2787,7 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t xml:space="preserve">   21 ( 10.8) </t>
+          <t xml:space="preserve">    21 ( 10.8) </t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
@@ -2804,7 +2804,7 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t xml:space="preserve">    0 (  0.0) </t>
+          <t xml:space="preserve">     0 (  0.0) </t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
@@ -2831,12 +2831,22 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t xml:space="preserve">  167 ( 86.1) </t>
+          <t xml:space="preserve">   167 ( 86.1) </t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
           <t xml:space="preserve">   161 (91.0) </t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0.192</t>
+        </is>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0.153</t>
         </is>
       </c>
     </row>
@@ -2853,22 +2863,12 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t xml:space="preserve">   27 ( 13.9) </t>
+          <t xml:space="preserve">    27 ( 13.9) </t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
           <t xml:space="preserve">    16 ( 9.0) </t>
-        </is>
-      </c>
-      <c r="F90" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0.192</t>
-        </is>
-      </c>
-      <c r="H90" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0.153</t>
         </is>
       </c>
     </row>
@@ -2890,7 +2890,7 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t xml:space="preserve">    0 (  0.0) </t>
+          <t xml:space="preserve">     0 (  0.0) </t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
@@ -2912,7 +2912,7 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t xml:space="preserve">    0 (  0.0) </t>
+          <t xml:space="preserve">     0 (  0.0) </t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
@@ -2934,7 +2934,7 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t xml:space="preserve">   18 (  9.3) </t>
+          <t xml:space="preserve">    18 (  9.3) </t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
@@ -2956,7 +2956,7 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t xml:space="preserve">   47 ( 24.2) </t>
+          <t xml:space="preserve">    47 ( 24.2) </t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
@@ -2988,7 +2988,7 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t xml:space="preserve">    0 (  0.0) </t>
+          <t xml:space="preserve">     0 (  0.0) </t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
@@ -3010,7 +3010,7 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t xml:space="preserve">   20 ( 10.3) </t>
+          <t xml:space="preserve">    20 ( 10.3) </t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
@@ -3032,7 +3032,7 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t xml:space="preserve">  109 ( 56.2) </t>
+          <t xml:space="preserve">   109 ( 56.2) </t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
@@ -3059,7 +3059,7 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t xml:space="preserve">   57 ( 29.4) </t>
+          <t xml:space="preserve">    57 ( 29.4) </t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
@@ -3091,7 +3091,7 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t xml:space="preserve">  121 ( 62.4) </t>
+          <t xml:space="preserve">   121 ( 62.4) </t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
@@ -3108,7 +3108,7 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t xml:space="preserve">   16 (  8.2) </t>
+          <t xml:space="preserve">    16 (  8.2) </t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
@@ -3135,7 +3135,7 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t xml:space="preserve">   54 ( 27.8) </t>
+          <t xml:space="preserve">    54 ( 27.8) </t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
@@ -3167,7 +3167,7 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t xml:space="preserve">   85 ( 43.8) </t>
+          <t xml:space="preserve">    85 ( 43.8) </t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
@@ -3184,7 +3184,7 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t xml:space="preserve">   55 ( 28.4) </t>
+          <t xml:space="preserve">    55 ( 28.4) </t>
         </is>
       </c>
       <c r="E103" t="inlineStr">

</xml_diff>

<commit_message>
Listo para analisis de competing risks
</commit_message>
<xml_diff>
--- a/Outputs/Tablas_basales/Tabla_basal_con_missings.xlsx
+++ b/Outputs/Tablas_basales/Tabla_basal_con_missings.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H105"/>
+  <dimension ref="A1:H109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1073,7 +1073,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>FsC_Elastografia (median [IQR])</t>
+          <t>FsC (median [IQR])</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1110,7 +1110,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>FsC_Elastografia (missing values)</t>
+          <t>FsC (missing values)</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1132,27 +1132,27 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>GGT_preIQ (median [IQR])</t>
+          <t>FsC_Elastografia (median [IQR])</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 75.50 [41.00, 130.50]</t>
+          <t xml:space="preserve"> 22.15 [14.10, 35.17]</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 74.00 [47.00, 113.00]</t>
+          <t xml:space="preserve"> 28.50 [18.90, 39.60]</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 77.00 [37.50, 140.00]</t>
+          <t xml:space="preserve"> 17.15 [11.83, 22.23]</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.467</t>
+          <t>&lt;0.001</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
@@ -1162,56 +1162,56 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.246</t>
+          <t xml:space="preserve"> 0.698</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>GGT_preIQ (missing values)</t>
+          <t>FsC_Elastografia (missing values)</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>47</t>
+          <t>189</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>37</t>
+          <t>90</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>99</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>HVPG_basal (median [IQR])</t>
+          <t>GGT_preIQ (median [IQR])</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 16.00 [12.62, 19.50]</t>
+          <t xml:space="preserve"> 75.50 [41.00, 130.50]</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 17.00 [14.00, 20.50]</t>
+          <t xml:space="preserve"> 74.00 [47.00, 113.00]</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 10.50 [6.00, 13.50]</t>
+          <t xml:space="preserve"> 77.00 [37.50, 140.00]</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>&lt;0.001</t>
+          <t xml:space="preserve"> 0.467</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
@@ -1221,56 +1221,56 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 1.434</t>
+          <t xml:space="preserve"> 0.246</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>HVPG_basal (missing values)</t>
+          <t>GGT_preIQ (missing values)</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>121</t>
+          <t>47</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>37</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>121</t>
+          <t>10</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>INR_preIQ (median [IQR])</t>
+          <t>HVPG_basal (median [IQR])</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t xml:space="preserve">  1.14 [1.06, 1.24]</t>
+          <t xml:space="preserve"> 16.00 [12.62, 19.50]</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t xml:space="preserve">  1.16 [1.09, 1.26]</t>
+          <t xml:space="preserve"> 17.00 [14.00, 20.50]</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t xml:space="preserve">  1.12 [1.03, 1.21]</t>
+          <t xml:space="preserve"> 10.50 [6.00, 13.50]</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.001</t>
+          <t>&lt;0.001</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
@@ -1280,56 +1280,56 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.177</t>
+          <t xml:space="preserve"> 1.434</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>INR_preIQ (missing values)</t>
+          <t>HVPG_basal (missing values)</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>121</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>121</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>K_preIQ (median [IQR])</t>
+          <t>INR_preIQ (median [IQR])</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t xml:space="preserve">  4.10 [4.00, 4.42]</t>
+          <t xml:space="preserve">  1.14 [1.06, 1.24]</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t xml:space="preserve">  4.00 [4.00, 4.20]</t>
+          <t xml:space="preserve">  1.16 [1.09, 1.26]</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t xml:space="preserve">  4.29 [3.93, 4.57]</t>
+          <t xml:space="preserve">  1.12 [1.03, 1.21]</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>&lt;0.001</t>
+          <t xml:space="preserve"> 0.001</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
@@ -1339,56 +1339,56 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.305</t>
+          <t xml:space="preserve"> 0.177</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>K_preIQ (missing values)</t>
+          <t>INR_preIQ (missing values)</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>38</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Leucos_preIQ (median [IQR])</t>
+          <t>K_preIQ (median [IQR])</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t xml:space="preserve">  6.58 [5.00, 8.19]</t>
+          <t xml:space="preserve">  4.10 [4.00, 4.42]</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t xml:space="preserve">    NA [NA, NA]</t>
+          <t xml:space="preserve">  4.00 [4.00, 4.20]</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t xml:space="preserve">  6.58 [5.00, 8.19]</t>
+          <t xml:space="preserve">  4.29 [3.93, 4.57]</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t xml:space="preserve">    NA</t>
+          <t>&lt;0.001</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
@@ -1398,41 +1398,41 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t xml:space="preserve">    NA</t>
+          <t xml:space="preserve"> 0.305</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Leucos_preIQ (missing values)</t>
+          <t>K_preIQ (missing values)</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>194</t>
+          <t>39</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>194</t>
+          <t>38</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>MELD_1anyspostIQ (median [IQR])</t>
+          <t>Leucos_preIQ (median [IQR])</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t xml:space="preserve">  8.00 [7.00, 11.00]</t>
+          <t xml:space="preserve">  6.58 [5.00, 8.19]</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1442,7 +1442,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t xml:space="preserve">  8.00 [7.00, 11.00]</t>
+          <t xml:space="preserve">  6.58 [5.00, 8.19]</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -1464,12 +1464,12 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>MELD_1anyspostIQ (missing values)</t>
+          <t>Leucos_preIQ (missing values)</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>221</t>
+          <t>194</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1479,34 +1479,34 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>MELD_basal (median [IQR])</t>
+          <t>MELD_1anyspostIQ (median [IQR])</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t xml:space="preserve">  8.90 [7.58, 10.34]</t>
+          <t xml:space="preserve">  8.00 [7.00, 11.00]</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t xml:space="preserve">  9.04 [7.91, 10.45]</t>
+          <t xml:space="preserve">    NA [NA, NA]</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t xml:space="preserve">  8.00 [7.00, 10.00]</t>
+          <t xml:space="preserve">  8.00 [7.00, 11.00]</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.005</t>
+          <t xml:space="preserve">    NA</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
@@ -1516,56 +1516,56 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.043</t>
+          <t xml:space="preserve">    NA</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>MELD_basal (missing values)</t>
+          <t>MELD_1anyspostIQ (missing values)</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>221</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>194</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>27</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>NA_preIQ_ (median [IQR])</t>
+          <t>MELD_basal (median [IQR])</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>140.00 [138.00, 142.00]</t>
+          <t xml:space="preserve">  8.90 [7.58, 10.34]</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>141.00 [139.00, 142.00]</t>
+          <t xml:space="preserve">  9.04 [7.91, 10.45]</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>139.00 [138.00, 141.00]</t>
+          <t xml:space="preserve">  8.00 [7.00, 10.00]</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>&lt;0.001</t>
+          <t xml:space="preserve"> 0.005</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
@@ -1575,24 +1575,24 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.388</t>
+          <t xml:space="preserve"> 0.043</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>NA_preIQ_ (missing values)</t>
+          <t>MELD_basal (missing values)</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -1604,27 +1604,27 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>PCR_preIQ (median [IQR])</t>
+          <t>NA_preIQ_ (median [IQR])</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t xml:space="preserve">  6.50 [3.30, 29.35]</t>
+          <t>140.00 [138.00, 142.00]</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t xml:space="preserve">    NA [NA, NA]</t>
+          <t>141.00 [139.00, 142.00]</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t xml:space="preserve">  6.50 [3.30, 29.35]</t>
+          <t>139.00 [138.00, 141.00]</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t xml:space="preserve">    NA</t>
+          <t>&lt;0.001</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
@@ -1634,56 +1634,56 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t xml:space="preserve">    NA</t>
+          <t xml:space="preserve"> 0.388</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>PCR_preIQ (missing values)</t>
+          <t>NA_preIQ_ (missing values)</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>304</t>
+          <t>39</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>194</t>
+          <t>39</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>110</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Pughpunts_basal (median [IQR])</t>
+          <t>PCR_preIQ (median [IQR])</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t xml:space="preserve">  5.00 [5.00, 6.00]</t>
+          <t xml:space="preserve">  6.50 [3.30, 29.35]</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t xml:space="preserve">  5.00 [5.00, 6.00]</t>
+          <t xml:space="preserve">    NA [NA, NA]</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t xml:space="preserve">  5.00 [5.00, 6.00]</t>
+          <t xml:space="preserve">  6.50 [3.30, 29.35]</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.536</t>
+          <t xml:space="preserve">    NA</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
@@ -1693,56 +1693,56 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.122</t>
+          <t xml:space="preserve">    NA</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Pughpunts_basal (missing values)</t>
+          <t>PCR_preIQ (missing values)</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>304</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>194</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>110</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Urea_mgdL_preIQ (median [IQR])</t>
+          <t>Pughpunts_basal (median [IQR])</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t xml:space="preserve">  9.30 [5.00, 37.00]</t>
+          <t xml:space="preserve">  5.00 [5.00, 6.00]</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t xml:space="preserve">  5.00 [4.00, 6.40]</t>
+          <t xml:space="preserve">  5.00 [5.00, 6.00]</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 38.00 [28.75, 47.80]</t>
+          <t xml:space="preserve">  5.00 [5.00, 6.00]</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>&lt;0.001</t>
+          <t xml:space="preserve"> 0.536</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
@@ -1752,51 +1752,51 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 2.354</t>
+          <t xml:space="preserve"> 0.122</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Urea_mgdL_preIQ (missing values)</t>
+          <t>Pughpunts_basal (missing values)</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
           <t>0</t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>5</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>plaquetes_preIQ (median [IQR])</t>
+          <t>Urea_mgdL_preIQ (median [IQR])</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>107.00 [80.00, 155.00]</t>
+          <t xml:space="preserve">  9.30 [5.00, 37.00]</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 95.00 [70.75, 123.00]</t>
+          <t xml:space="preserve">  5.00 [4.00, 6.40]</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>134.00 [100.00, 180.00]</t>
+          <t xml:space="preserve"> 38.00 [28.75, 47.80]</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -1811,1238 +1811,1258 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.753</t>
+          <t xml:space="preserve"> 2.354</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>plaquetes_preIQ (missing values)</t>
+          <t>Urea_mgdL_preIQ (missing values)</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>DIabetes (%)</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>insulina</t>
+          <t>hvpg (median [IQR])</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t xml:space="preserve">   126 (34.0) </t>
+          <t xml:space="preserve"> 16.00 [12.62, 19.50]</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t xml:space="preserve">    67 ( 34.5) </t>
+          <t xml:space="preserve"> 17.00 [14.00, 20.50]</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t xml:space="preserve">    59 (33.3) </t>
+          <t xml:space="preserve"> 10.50 [6.00, 13.50]</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>&lt;0.001</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>nonnorm</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1.434</t>
         </is>
       </c>
     </row>
     <row r="52">
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>no</t>
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>hvpg (missing values)</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t xml:space="preserve">   244 (65.8) </t>
+          <t>121</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t xml:space="preserve">   126 ( 64.9) </t>
+          <t>0</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t xml:space="preserve">   118 (66.7) </t>
-        </is>
-      </c>
-      <c r="F52" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0.609</t>
-        </is>
-      </c>
-      <c r="H52" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0.106</t>
+          <t>121</t>
         </is>
       </c>
     </row>
     <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>plaquetes_preIQ (median [IQR])</t>
+        </is>
+      </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t xml:space="preserve">     1 ( 0.3) </t>
+          <t>107.00 [80.00, 155.00]</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t xml:space="preserve">     1 (  0.5) </t>
+          <t xml:space="preserve"> 95.00 [70.75, 123.00]</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t xml:space="preserve">     0 ( 0.0) </t>
+          <t>134.00 [100.00, 180.00]</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>&lt;0.001</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>nonnorm</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0.753</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
+          <t>plaquetes_preIQ (missing values)</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>DIabetes (%)</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>insulina</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   126 (34.0) </t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    67 ( 34.5) </t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    59 (33.3) </t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   244 (65.8) </t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   126 ( 64.9) </t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   118 (66.7) </t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0.609</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0.106</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="C57" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     1 ( 0.3) </t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     1 (  0.5) </t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     0 ( 0.0) </t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
           <t>Enol_Actiu (%)</t>
         </is>
       </c>
-      <c r="B54" t="inlineStr">
+      <c r="B58" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="C54" t="inlineStr">
+      <c r="C58" t="inlineStr">
         <is>
           <t xml:space="preserve">   308 (83.0) </t>
         </is>
       </c>
-      <c r="D54" t="inlineStr">
+      <c r="D58" t="inlineStr">
         <is>
           <t xml:space="preserve">   158 ( 81.4) </t>
         </is>
       </c>
-      <c r="E54" t="inlineStr">
+      <c r="E58" t="inlineStr">
         <is>
           <t xml:space="preserve">   150 (84.7) </t>
         </is>
       </c>
-      <c r="F54" t="inlineStr">
+      <c r="F58" t="inlineStr">
         <is>
           <t xml:space="preserve"> 0.479</t>
         </is>
       </c>
-      <c r="H54" t="inlineStr">
+      <c r="H58" t="inlineStr">
         <is>
           <t xml:space="preserve"> 0.088</t>
         </is>
       </c>
     </row>
-    <row r="55">
-      <c r="B55" t="inlineStr">
+    <row r="59">
+      <c r="B59" t="inlineStr">
         <is>
           <t>si</t>
         </is>
       </c>
-      <c r="C55" t="inlineStr">
+      <c r="C59" t="inlineStr">
         <is>
           <t xml:space="preserve">    63 (17.0) </t>
         </is>
       </c>
-      <c r="D55" t="inlineStr">
+      <c r="D59" t="inlineStr">
         <is>
           <t xml:space="preserve">    36 ( 18.6) </t>
         </is>
       </c>
-      <c r="E55" t="inlineStr">
+      <c r="E59" t="inlineStr">
         <is>
           <t xml:space="preserve">    27 (15.3) </t>
         </is>
       </c>
     </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
+    <row r="60">
+      <c r="A60" t="inlineStr">
         <is>
           <t>FsC_10 (%)</t>
         </is>
       </c>
-      <c r="B56" t="inlineStr">
+      <c r="B60" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="C56" t="inlineStr">
+      <c r="C60" t="inlineStr">
         <is>
           <t xml:space="preserve">    15 ( 4.0) </t>
         </is>
       </c>
-      <c r="D56" t="inlineStr">
+      <c r="D60" t="inlineStr">
         <is>
           <t xml:space="preserve">     1 (  0.5) </t>
         </is>
       </c>
-      <c r="E56" t="inlineStr">
+      <c r="E60" t="inlineStr">
         <is>
           <t xml:space="preserve">    14 ( 7.9) </t>
         </is>
       </c>
-      <c r="F56" t="inlineStr">
+      <c r="F60" t="inlineStr">
         <is>
           <t>&lt;0.001</t>
         </is>
       </c>
-      <c r="H56" t="inlineStr">
+      <c r="H60" t="inlineStr">
         <is>
           <t xml:space="preserve"> 0.473</t>
         </is>
       </c>
     </row>
-    <row r="57">
-      <c r="B57" t="inlineStr">
+    <row r="61">
+      <c r="B61" t="inlineStr">
         <is>
           <t>si</t>
         </is>
       </c>
-      <c r="C57" t="inlineStr">
+      <c r="C61" t="inlineStr">
         <is>
           <t xml:space="preserve">   167 (45.0) </t>
         </is>
       </c>
-      <c r="D57" t="inlineStr">
+      <c r="D61" t="inlineStr">
         <is>
           <t xml:space="preserve">   103 ( 53.1) </t>
         </is>
       </c>
-      <c r="E57" t="inlineStr">
+      <c r="E61" t="inlineStr">
         <is>
           <t xml:space="preserve">    64 (36.2) </t>
         </is>
       </c>
     </row>
-    <row r="58">
-      <c r="C58" t="inlineStr">
+    <row r="62">
+      <c r="C62" t="inlineStr">
         <is>
           <t xml:space="preserve">   189 (50.9) </t>
         </is>
       </c>
-      <c r="D58" t="inlineStr">
+      <c r="D62" t="inlineStr">
         <is>
           <t xml:space="preserve">    90 ( 46.4) </t>
         </is>
       </c>
-      <c r="E58" t="inlineStr">
+      <c r="E62" t="inlineStr">
         <is>
           <t xml:space="preserve">    99 (55.9) </t>
         </is>
       </c>
     </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
+    <row r="63">
+      <c r="A63" t="inlineStr">
         <is>
           <t>FsC_15 (%)</t>
         </is>
       </c>
-      <c r="B59" t="inlineStr">
+      <c r="B63" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="C59" t="inlineStr">
+      <c r="C63" t="inlineStr">
         <is>
           <t xml:space="preserve">    51 (13.7) </t>
         </is>
       </c>
-      <c r="D59" t="inlineStr">
+      <c r="D63" t="inlineStr">
         <is>
           <t xml:space="preserve">    17 (  8.8) </t>
         </is>
       </c>
-      <c r="E59" t="inlineStr">
+      <c r="E63" t="inlineStr">
         <is>
           <t xml:space="preserve">    34 (19.2) </t>
         </is>
       </c>
-      <c r="F59" t="inlineStr">
+      <c r="F63" t="inlineStr">
         <is>
           <t>&lt;0.001</t>
         </is>
       </c>
-      <c r="H59" t="inlineStr">
+      <c r="H63" t="inlineStr">
         <is>
           <t xml:space="preserve"> 0.471</t>
         </is>
       </c>
     </row>
-    <row r="60">
-      <c r="B60" t="inlineStr">
+    <row r="64">
+      <c r="B64" t="inlineStr">
         <is>
           <t>si</t>
         </is>
       </c>
-      <c r="C60" t="inlineStr">
+      <c r="C64" t="inlineStr">
         <is>
           <t xml:space="preserve">   131 (35.3) </t>
         </is>
       </c>
-      <c r="D60" t="inlineStr">
+      <c r="D64" t="inlineStr">
         <is>
           <t xml:space="preserve">    87 ( 44.8) </t>
         </is>
       </c>
-      <c r="E60" t="inlineStr">
+      <c r="E64" t="inlineStr">
         <is>
           <t xml:space="preserve">    44 (24.9) </t>
         </is>
       </c>
     </row>
-    <row r="61">
-      <c r="C61" t="inlineStr">
+    <row r="65">
+      <c r="C65" t="inlineStr">
         <is>
           <t xml:space="preserve">   189 (50.9) </t>
         </is>
       </c>
-      <c r="D61" t="inlineStr">
+      <c r="D65" t="inlineStr">
         <is>
           <t xml:space="preserve">    90 ( 46.4) </t>
         </is>
       </c>
-      <c r="E61" t="inlineStr">
+      <c r="E65" t="inlineStr">
         <is>
           <t xml:space="preserve">    99 (55.9) </t>
         </is>
       </c>
     </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
+    <row r="66">
+      <c r="A66" t="inlineStr">
         <is>
           <t>FsC_25 (%)</t>
         </is>
       </c>
-      <c r="B62" t="inlineStr">
+      <c r="B66" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="C62" t="inlineStr">
+      <c r="C66" t="inlineStr">
         <is>
           <t xml:space="preserve">   103 (27.8) </t>
         </is>
       </c>
-      <c r="D62" t="inlineStr">
+      <c r="D66" t="inlineStr">
         <is>
           <t xml:space="preserve">    43 ( 22.2) </t>
         </is>
       </c>
-      <c r="E62" t="inlineStr">
+      <c r="E66" t="inlineStr">
         <is>
           <t xml:space="preserve">    60 (33.9) </t>
         </is>
       </c>
-      <c r="F62" t="inlineStr">
+      <c r="F66" t="inlineStr">
         <is>
           <t>&lt;0.001</t>
         </is>
       </c>
-      <c r="H62" t="inlineStr">
+      <c r="H66" t="inlineStr">
         <is>
           <t xml:space="preserve"> 0.553</t>
         </is>
       </c>
     </row>
-    <row r="63">
-      <c r="B63" t="inlineStr">
+    <row r="67">
+      <c r="B67" t="inlineStr">
         <is>
           <t>si</t>
         </is>
       </c>
-      <c r="C63" t="inlineStr">
+      <c r="C67" t="inlineStr">
         <is>
           <t xml:space="preserve">    79 (21.3) </t>
         </is>
       </c>
-      <c r="D63" t="inlineStr">
+      <c r="D67" t="inlineStr">
         <is>
           <t xml:space="preserve">    61 ( 31.4) </t>
         </is>
       </c>
-      <c r="E63" t="inlineStr">
+      <c r="E67" t="inlineStr">
         <is>
           <t xml:space="preserve">    18 (10.2) </t>
         </is>
       </c>
     </row>
-    <row r="64">
-      <c r="C64" t="inlineStr">
+    <row r="68">
+      <c r="C68" t="inlineStr">
         <is>
           <t xml:space="preserve">   189 (50.9) </t>
         </is>
       </c>
-      <c r="D64" t="inlineStr">
+      <c r="D68" t="inlineStr">
         <is>
           <t xml:space="preserve">    90 ( 46.4) </t>
         </is>
       </c>
-      <c r="E64" t="inlineStr">
+      <c r="E68" t="inlineStr">
         <is>
           <t xml:space="preserve">    99 (55.9) </t>
         </is>
       </c>
     </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
+    <row r="69">
+      <c r="A69" t="inlineStr">
         <is>
           <t>HCC_prev (%)</t>
         </is>
       </c>
-      <c r="B65" t="inlineStr">
+      <c r="B69" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="C65" t="inlineStr">
+      <c r="C69" t="inlineStr">
         <is>
           <t xml:space="preserve">   329 (88.7) </t>
         </is>
       </c>
-      <c r="D65" t="inlineStr">
+      <c r="D69" t="inlineStr">
         <is>
           <t xml:space="preserve">   188 ( 96.9) </t>
         </is>
       </c>
-      <c r="E65" t="inlineStr">
+      <c r="E69" t="inlineStr">
         <is>
           <t xml:space="preserve">   141 (79.7) </t>
         </is>
       </c>
-      <c r="F65" t="inlineStr">
+      <c r="F69" t="inlineStr">
         <is>
           <t>&lt;0.001</t>
         </is>
       </c>
-      <c r="H65" t="inlineStr">
+      <c r="H69" t="inlineStr">
         <is>
           <t xml:space="preserve"> 0.557</t>
         </is>
       </c>
     </row>
-    <row r="66">
-      <c r="B66" t="inlineStr">
+    <row r="70">
+      <c r="B70" t="inlineStr">
         <is>
           <t>si</t>
         </is>
       </c>
-      <c r="C66" t="inlineStr">
+      <c r="C70" t="inlineStr">
         <is>
           <t xml:space="preserve">    42 (11.3) </t>
         </is>
       </c>
-      <c r="D66" t="inlineStr">
+      <c r="D70" t="inlineStr">
         <is>
           <t xml:space="preserve">     6 (  3.1) </t>
         </is>
       </c>
-      <c r="E66" t="inlineStr">
+      <c r="E70" t="inlineStr">
         <is>
           <t xml:space="preserve">    36 (20.3) </t>
         </is>
       </c>
     </row>
-    <row r="67">
-      <c r="A67" t="inlineStr">
+    <row r="71">
+      <c r="A71" t="inlineStr">
         <is>
           <t>HTA (%)</t>
         </is>
       </c>
-      <c r="B67" t="inlineStr">
+      <c r="B71" t="inlineStr">
         <is>
           <t>IECA</t>
         </is>
       </c>
-      <c r="C67" t="inlineStr">
+      <c r="C71" t="inlineStr">
         <is>
           <t xml:space="preserve">   193 (52.0) </t>
         </is>
       </c>
-      <c r="D67" t="inlineStr">
+      <c r="D71" t="inlineStr">
         <is>
           <t xml:space="preserve">    86 ( 44.3) </t>
         </is>
       </c>
-      <c r="E67" t="inlineStr">
+      <c r="E71" t="inlineStr">
         <is>
           <t xml:space="preserve">   107 (60.5) </t>
         </is>
       </c>
     </row>
-    <row r="68">
-      <c r="B68" t="inlineStr">
+    <row r="72">
+      <c r="B72" t="inlineStr">
         <is>
           <t>ninguno</t>
         </is>
       </c>
-      <c r="C68" t="inlineStr">
+      <c r="C72" t="inlineStr">
         <is>
           <t xml:space="preserve">   175 (47.2) </t>
         </is>
       </c>
-      <c r="D68" t="inlineStr">
+      <c r="D72" t="inlineStr">
         <is>
           <t xml:space="preserve">   105 ( 54.1) </t>
         </is>
       </c>
-      <c r="E68" t="inlineStr">
+      <c r="E72" t="inlineStr">
         <is>
           <t xml:space="preserve">    70 (39.5) </t>
         </is>
       </c>
-      <c r="F68" t="inlineStr">
+      <c r="F72" t="inlineStr">
         <is>
           <t xml:space="preserve"> 0.003</t>
         </is>
       </c>
-      <c r="H68" t="inlineStr">
+      <c r="H72" t="inlineStr">
         <is>
           <t xml:space="preserve"> 0.361</t>
         </is>
       </c>
     </row>
-    <row r="69">
-      <c r="C69" t="inlineStr">
+    <row r="73">
+      <c r="C73" t="inlineStr">
         <is>
           <t xml:space="preserve">     3 ( 0.8) </t>
         </is>
       </c>
-      <c r="D69" t="inlineStr">
+      <c r="D73" t="inlineStr">
         <is>
           <t xml:space="preserve">     3 (  1.5) </t>
         </is>
       </c>
-      <c r="E69" t="inlineStr">
+      <c r="E73" t="inlineStr">
         <is>
           <t xml:space="preserve">     0 ( 0.0) </t>
         </is>
       </c>
     </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
+    <row r="74">
+      <c r="A74" t="inlineStr">
         <is>
           <t>HVPG_10 (%)</t>
         </is>
       </c>
-      <c r="B70" t="inlineStr">
+      <c r="B74" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="C70" t="inlineStr">
+      <c r="C74" t="inlineStr">
         <is>
           <t xml:space="preserve">    29 ( 7.8) </t>
         </is>
       </c>
-      <c r="D70" t="inlineStr">
+      <c r="D74" t="inlineStr">
         <is>
           <t xml:space="preserve">     0 (  0.0) </t>
         </is>
       </c>
-      <c r="E70" t="inlineStr">
+      <c r="E74" t="inlineStr">
         <is>
           <t xml:space="preserve">    29 (16.4) </t>
         </is>
       </c>
-      <c r="F70" t="inlineStr">
+      <c r="F74" t="inlineStr">
         <is>
           <t>&lt;0.001</t>
         </is>
       </c>
-      <c r="H70" t="inlineStr">
+      <c r="H74" t="inlineStr">
         <is>
           <t xml:space="preserve"> 3.333</t>
         </is>
       </c>
     </row>
-    <row r="71">
-      <c r="B71" t="inlineStr">
+    <row r="75">
+      <c r="B75" t="inlineStr">
         <is>
           <t>si</t>
         </is>
       </c>
-      <c r="C71" t="inlineStr">
+      <c r="C75" t="inlineStr">
         <is>
           <t xml:space="preserve">   221 (59.6) </t>
         </is>
       </c>
-      <c r="D71" t="inlineStr">
+      <c r="D75" t="inlineStr">
         <is>
           <t xml:space="preserve">   194 (100.0) </t>
         </is>
       </c>
-      <c r="E71" t="inlineStr">
+      <c r="E75" t="inlineStr">
         <is>
           <t xml:space="preserve">    27 (15.3) </t>
         </is>
       </c>
     </row>
-    <row r="72">
-      <c r="C72" t="inlineStr">
+    <row r="76">
+      <c r="C76" t="inlineStr">
         <is>
           <t xml:space="preserve">   121 (32.6) </t>
         </is>
       </c>
-      <c r="D72" t="inlineStr">
+      <c r="D76" t="inlineStr">
         <is>
           <t xml:space="preserve">     0 (  0.0) </t>
         </is>
       </c>
-      <c r="E72" t="inlineStr">
+      <c r="E76" t="inlineStr">
         <is>
           <t xml:space="preserve">   121 (68.4) </t>
         </is>
       </c>
     </row>
-    <row r="73">
-      <c r="A73" t="inlineStr">
+    <row r="77">
+      <c r="A77" t="inlineStr">
         <is>
           <t>HVPG_16 (%)</t>
         </is>
       </c>
-      <c r="B73" t="inlineStr">
+      <c r="B77" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="C73" t="inlineStr">
+      <c r="C77" t="inlineStr">
         <is>
           <t xml:space="preserve">   116 (31.3) </t>
         </is>
       </c>
-      <c r="D73" t="inlineStr">
+      <c r="D77" t="inlineStr">
         <is>
           <t xml:space="preserve">    70 ( 36.1) </t>
         </is>
       </c>
-      <c r="E73" t="inlineStr">
+      <c r="E77" t="inlineStr">
         <is>
           <t xml:space="preserve">    46 (26.0) </t>
         </is>
       </c>
-      <c r="F73" t="inlineStr">
+      <c r="F77" t="inlineStr">
         <is>
           <t>&lt;0.001</t>
         </is>
       </c>
-      <c r="H73" t="inlineStr">
+      <c r="H77" t="inlineStr">
         <is>
           <t xml:space="preserve"> 2.419</t>
         </is>
       </c>
     </row>
-    <row r="74">
-      <c r="B74" t="inlineStr">
+    <row r="78">
+      <c r="B78" t="inlineStr">
         <is>
           <t>si</t>
         </is>
       </c>
-      <c r="C74" t="inlineStr">
+      <c r="C78" t="inlineStr">
         <is>
           <t xml:space="preserve">   134 (36.1) </t>
         </is>
       </c>
-      <c r="D74" t="inlineStr">
+      <c r="D78" t="inlineStr">
         <is>
           <t xml:space="preserve">   124 ( 63.9) </t>
         </is>
       </c>
-      <c r="E74" t="inlineStr">
+      <c r="E78" t="inlineStr">
         <is>
           <t xml:space="preserve">    10 ( 5.6) </t>
         </is>
       </c>
     </row>
-    <row r="75">
-      <c r="C75" t="inlineStr">
+    <row r="79">
+      <c r="C79" t="inlineStr">
         <is>
           <t xml:space="preserve">   121 (32.6) </t>
         </is>
       </c>
-      <c r="D75" t="inlineStr">
+      <c r="D79" t="inlineStr">
         <is>
           <t xml:space="preserve">     0 (  0.0) </t>
         </is>
       </c>
-      <c r="E75" t="inlineStr">
+      <c r="E79" t="inlineStr">
         <is>
           <t xml:space="preserve">   121 (68.4) </t>
         </is>
       </c>
     </row>
-    <row r="76">
-      <c r="A76" t="inlineStr">
+    <row r="80">
+      <c r="A80" t="inlineStr">
         <is>
           <t>HVPG_20 (%)</t>
         </is>
       </c>
-      <c r="B76" t="inlineStr">
+      <c r="B80" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="C76" t="inlineStr">
+      <c r="C80" t="inlineStr">
         <is>
           <t xml:space="preserve">   188 (50.7) </t>
         </is>
       </c>
-      <c r="D76" t="inlineStr">
+      <c r="D80" t="inlineStr">
         <is>
           <t xml:space="preserve">   136 ( 70.1) </t>
         </is>
       </c>
-      <c r="E76" t="inlineStr">
+      <c r="E80" t="inlineStr">
         <is>
           <t xml:space="preserve">    52 (29.4) </t>
         </is>
       </c>
-      <c r="F76" t="inlineStr">
+      <c r="F80" t="inlineStr">
         <is>
           <t>&lt;0.001</t>
         </is>
       </c>
-      <c r="H76" t="inlineStr">
+      <c r="H80" t="inlineStr">
         <is>
           <t xml:space="preserve"> 2.184</t>
-        </is>
-      </c>
-    </row>
-    <row r="77">
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>si</t>
-        </is>
-      </c>
-      <c r="C77" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    62 (16.7) </t>
-        </is>
-      </c>
-      <c r="D77" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    58 ( 29.9) </t>
-        </is>
-      </c>
-      <c r="E77" t="inlineStr">
-        <is>
-          <t xml:space="preserve">     4 ( 2.3) </t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="C78" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   121 (32.6) </t>
-        </is>
-      </c>
-      <c r="D78" t="inlineStr">
-        <is>
-          <t xml:space="preserve">     0 (  0.0) </t>
-        </is>
-      </c>
-      <c r="E78" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   121 (68.4) </t>
-        </is>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>Pughclasse_basal (%)</t>
-        </is>
-      </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>pugh A</t>
-        </is>
-      </c>
-      <c r="C79" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   319 (86.0) </t>
-        </is>
-      </c>
-      <c r="D79" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   166 ( 85.6) </t>
-        </is>
-      </c>
-      <c r="E79" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   153 (86.4) </t>
-        </is>
-      </c>
-      <c r="F79" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0.352</t>
-        </is>
-      </c>
-      <c r="H79" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0.187</t>
-        </is>
-      </c>
-    </row>
-    <row r="80">
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>pugh B</t>
-        </is>
-      </c>
-      <c r="C80" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    49 (13.2) </t>
-        </is>
-      </c>
-      <c r="D80" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    27 ( 13.9) </t>
-        </is>
-      </c>
-      <c r="E80" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    22 (12.4) </t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="B81" t="inlineStr">
         <is>
-          <t>pugh C</t>
+          <t>si</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t xml:space="preserve">     2 ( 0.5) </t>
+          <t xml:space="preserve">    62 (16.7) </t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t xml:space="preserve">     0 (  0.0) </t>
+          <t xml:space="preserve">    58 ( 29.9) </t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t xml:space="preserve">     2 ( 1.1) </t>
+          <t xml:space="preserve">     4 ( 2.3) </t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="C82" t="inlineStr">
         <is>
-          <t xml:space="preserve">     1 ( 0.3) </t>
+          <t xml:space="preserve">   121 (32.6) </t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t xml:space="preserve">     1 (  0.5) </t>
+          <t xml:space="preserve">     0 (  0.0) </t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t xml:space="preserve">     0 ( 0.0) </t>
+          <t xml:space="preserve">   121 (68.4) </t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>SignesIndirectes_HTP (%)</t>
+          <t>Pughclasse_basal (%)</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>pugh A</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t xml:space="preserve">    64 (17.3) </t>
+          <t xml:space="preserve">   319 (86.0) </t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t xml:space="preserve">     3 (  1.5) </t>
+          <t xml:space="preserve">   166 ( 85.6) </t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t xml:space="preserve">    61 (34.5) </t>
+          <t xml:space="preserve">   153 (86.4) </t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>&lt;0.001</t>
+          <t xml:space="preserve"> 0.352</t>
         </is>
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.948</t>
+          <t xml:space="preserve"> 0.187</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="B84" t="inlineStr">
         <is>
+          <t>pugh B</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    49 (13.2) </t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    27 ( 13.9) </t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    22 (12.4) </t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>pugh C</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     2 ( 0.5) </t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     0 (  0.0) </t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     2 ( 1.1) </t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="C86" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     1 ( 0.3) </t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     1 (  0.5) </t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     0 ( 0.0) </t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>SignesIndirectes_HTP (%)</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    64 (17.3) </t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     3 (  1.5) </t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    61 (34.5) </t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>&lt;0.001</t>
+        </is>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0.948</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="B88" t="inlineStr">
+        <is>
           <t>si</t>
         </is>
       </c>
-      <c r="C84" t="inlineStr">
+      <c r="C88" t="inlineStr">
         <is>
           <t xml:space="preserve">   307 (82.7) </t>
         </is>
       </c>
-      <c r="D84" t="inlineStr">
+      <c r="D88" t="inlineStr">
         <is>
           <t xml:space="preserve">   191 ( 98.5) </t>
         </is>
       </c>
-      <c r="E84" t="inlineStr">
+      <c r="E88" t="inlineStr">
         <is>
           <t xml:space="preserve">   116 (65.5) </t>
         </is>
       </c>
     </row>
-    <row r="85">
-      <c r="A85" t="inlineStr">
+    <row r="89">
+      <c r="A89" t="inlineStr">
         <is>
           <t>VE_basal (%)</t>
         </is>
       </c>
-      <c r="B85" t="inlineStr">
+      <c r="B89" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="C85" t="inlineStr">
+      <c r="C89" t="inlineStr">
         <is>
           <t xml:space="preserve">   122 (32.9) </t>
         </is>
       </c>
-      <c r="D85" t="inlineStr">
+      <c r="D89" t="inlineStr">
         <is>
           <t xml:space="preserve">     3 (  1.5) </t>
         </is>
       </c>
-      <c r="E85" t="inlineStr">
+      <c r="E89" t="inlineStr">
         <is>
           <t xml:space="preserve">   119 (67.2) </t>
         </is>
       </c>
-      <c r="F85" t="inlineStr">
+      <c r="F89" t="inlineStr">
         <is>
           <t>&lt;0.001</t>
         </is>
       </c>
-      <c r="H85" t="inlineStr">
+      <c r="H89" t="inlineStr">
         <is>
           <t xml:space="preserve"> 2.187</t>
         </is>
       </c>
     </row>
-    <row r="86">
-      <c r="B86" t="inlineStr">
+    <row r="90">
+      <c r="B90" t="inlineStr">
         <is>
           <t>si</t>
         </is>
       </c>
-      <c r="C86" t="inlineStr">
+      <c r="C90" t="inlineStr">
         <is>
           <t xml:space="preserve">   239 (64.4) </t>
         </is>
       </c>
-      <c r="D86" t="inlineStr">
+      <c r="D90" t="inlineStr">
         <is>
           <t xml:space="preserve">   191 ( 98.5) </t>
         </is>
       </c>
-      <c r="E86" t="inlineStr">
+      <c r="E90" t="inlineStr">
         <is>
           <t xml:space="preserve">    48 (27.1) </t>
         </is>
       </c>
     </row>
-    <row r="87">
-      <c r="C87" t="inlineStr">
+    <row r="91">
+      <c r="C91" t="inlineStr">
         <is>
           <t xml:space="preserve">    10 ( 2.7) </t>
         </is>
       </c>
-      <c r="D87" t="inlineStr">
+      <c r="D91" t="inlineStr">
         <is>
           <t xml:space="preserve">     0 (  0.0) </t>
         </is>
       </c>
-      <c r="E87" t="inlineStr">
+      <c r="E91" t="inlineStr">
         <is>
           <t xml:space="preserve">    10 ( 5.6) </t>
         </is>
       </c>
     </row>
-    <row r="88">
-      <c r="A88" t="inlineStr">
+    <row r="92">
+      <c r="A92" t="inlineStr">
         <is>
           <t>VG_fúndiques (%)</t>
         </is>
       </c>
-      <c r="B88" t="inlineStr">
+      <c r="B92" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="C88" t="inlineStr">
+      <c r="C92" t="inlineStr">
         <is>
           <t xml:space="preserve">   332 (89.5) </t>
         </is>
       </c>
-      <c r="D88" t="inlineStr">
+      <c r="D92" t="inlineStr">
         <is>
           <t xml:space="preserve">   173 ( 89.2) </t>
         </is>
       </c>
-      <c r="E88" t="inlineStr">
+      <c r="E92" t="inlineStr">
         <is>
           <t xml:space="preserve">   159 (89.8) </t>
         </is>
       </c>
-      <c r="F88" t="inlineStr">
+      <c r="F92" t="inlineStr">
         <is>
           <t>&lt;0.001</t>
         </is>
       </c>
-      <c r="H88" t="inlineStr">
+      <c r="H92" t="inlineStr">
         <is>
           <t xml:space="preserve"> 0.444</t>
         </is>
       </c>
     </row>
-    <row r="89">
-      <c r="B89" t="inlineStr">
+    <row r="93">
+      <c r="B93" t="inlineStr">
         <is>
           <t>si</t>
         </is>
       </c>
-      <c r="C89" t="inlineStr">
+      <c r="C93" t="inlineStr">
         <is>
           <t xml:space="preserve">    28 ( 7.5) </t>
         </is>
       </c>
-      <c r="D89" t="inlineStr">
+      <c r="D93" t="inlineStr">
         <is>
           <t xml:space="preserve">    21 ( 10.8) </t>
         </is>
       </c>
-      <c r="E89" t="inlineStr">
+      <c r="E93" t="inlineStr">
         <is>
           <t xml:space="preserve">     7 ( 4.0) </t>
         </is>
       </c>
     </row>
-    <row r="90">
-      <c r="C90" t="inlineStr">
+    <row r="94">
+      <c r="C94" t="inlineStr">
         <is>
           <t xml:space="preserve">    11 ( 3.0) </t>
         </is>
       </c>
-      <c r="D90" t="inlineStr">
+      <c r="D94" t="inlineStr">
         <is>
           <t xml:space="preserve">     0 (  0.0) </t>
         </is>
       </c>
-      <c r="E90" t="inlineStr">
+      <c r="E94" t="inlineStr">
         <is>
           <t xml:space="preserve">    11 ( 6.2) </t>
         </is>
       </c>
     </row>
-    <row r="91">
-      <c r="A91" t="inlineStr">
+    <row r="95">
+      <c r="A95" t="inlineStr">
         <is>
           <t>dislipemias (%)</t>
         </is>
       </c>
-      <c r="B91" t="inlineStr">
+      <c r="B95" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="C91" t="inlineStr">
+      <c r="C95" t="inlineStr">
         <is>
           <t xml:space="preserve">   328 (88.4) </t>
         </is>
       </c>
-      <c r="D91" t="inlineStr">
+      <c r="D95" t="inlineStr">
         <is>
           <t xml:space="preserve">   167 ( 86.1) </t>
         </is>
       </c>
-      <c r="E91" t="inlineStr">
+      <c r="E95" t="inlineStr">
         <is>
           <t xml:space="preserve">   161 (91.0) </t>
         </is>
       </c>
-      <c r="F91" t="inlineStr">
+      <c r="F95" t="inlineStr">
         <is>
           <t xml:space="preserve"> 0.192</t>
         </is>
       </c>
-      <c r="H91" t="inlineStr">
+      <c r="H95" t="inlineStr">
         <is>
           <t xml:space="preserve"> 0.153</t>
-        </is>
-      </c>
-    </row>
-    <row r="92">
-      <c r="B92" t="inlineStr">
-        <is>
-          <t>Si</t>
-        </is>
-      </c>
-      <c r="C92" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    43 (11.6) </t>
-        </is>
-      </c>
-      <c r="D92" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    27 ( 13.9) </t>
-        </is>
-      </c>
-      <c r="E92" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    16 ( 9.0) </t>
-        </is>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="inlineStr">
-        <is>
-          <t>etiologiaCH (%)</t>
-        </is>
-      </c>
-      <c r="B93" t="inlineStr">
-        <is>
-          <t>Altres</t>
-        </is>
-      </c>
-      <c r="C93" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    17 ( 4.6) </t>
-        </is>
-      </c>
-      <c r="D93" t="inlineStr">
-        <is>
-          <t xml:space="preserve">     0 (  0.0) </t>
-        </is>
-      </c>
-      <c r="E93" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    17 ( 9.6) </t>
-        </is>
-      </c>
-    </row>
-    <row r="94">
-      <c r="B94" t="inlineStr">
-        <is>
-          <t>Colestàtica?/Autoimmune</t>
-        </is>
-      </c>
-      <c r="C94" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    10 ( 2.7) </t>
-        </is>
-      </c>
-      <c r="D94" t="inlineStr">
-        <is>
-          <t xml:space="preserve">     0 (  0.0) </t>
-        </is>
-      </c>
-      <c r="E94" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    10 ( 5.6) </t>
-        </is>
-      </c>
-    </row>
-    <row r="95">
-      <c r="B95" t="inlineStr">
-        <is>
-          <t>MAFLD</t>
-        </is>
-      </c>
-      <c r="C95" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    39 (10.5) </t>
-        </is>
-      </c>
-      <c r="D95" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    18 (  9.3) </t>
-        </is>
-      </c>
-      <c r="E95" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    21 (11.9) </t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="B96" t="inlineStr">
         <is>
-          <t>OH</t>
+          <t>Si</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t xml:space="preserve">    76 (20.5) </t>
+          <t xml:space="preserve">    43 (11.6) </t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t xml:space="preserve">    47 ( 24.2) </t>
+          <t xml:space="preserve">    27 ( 13.9) </t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t xml:space="preserve">    29 (16.4) </t>
-        </is>
-      </c>
-      <c r="F96" t="inlineStr">
-        <is>
-          <t>&lt;0.001</t>
-        </is>
-      </c>
-      <c r="H96" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0.778</t>
+          <t xml:space="preserve">    16 ( 9.0) </t>
         </is>
       </c>
     </row>
     <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>etiologiaCH (%)</t>
+        </is>
+      </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>OH+MAFLD</t>
+          <t>Altres</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t xml:space="preserve">     9 ( 2.4) </t>
+          <t xml:space="preserve">    17 ( 4.6) </t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
@@ -3052,63 +3072,58 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t xml:space="preserve">     9 ( 5.1) </t>
+          <t xml:space="preserve">    17 ( 9.6) </t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="B98" t="inlineStr">
         <is>
-          <t>OH+Virus</t>
+          <t>Colestàtica?/Autoimmune</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t xml:space="preserve">    26 ( 7.0) </t>
+          <t xml:space="preserve">    10 ( 2.7) </t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t xml:space="preserve">    20 ( 10.3) </t>
+          <t xml:space="preserve">     0 (  0.0) </t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t xml:space="preserve">     6 ( 3.4) </t>
+          <t xml:space="preserve">    10 ( 5.6) </t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="B99" t="inlineStr">
         <is>
-          <t>Virus</t>
+          <t>MAFLD</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t xml:space="preserve">   194 (52.3) </t>
+          <t xml:space="preserve">    39 (10.5) </t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t xml:space="preserve">   109 ( 56.2) </t>
+          <t xml:space="preserve">    18 (  9.3) </t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t xml:space="preserve">    85 (48.0) </t>
+          <t xml:space="preserve">    21 (11.9) </t>
         </is>
       </c>
     </row>
     <row r="100">
-      <c r="A100" t="inlineStr">
-        <is>
-          <t>respostHDK_aguda (%)</t>
-        </is>
-      </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>OH</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -3118,12 +3133,12 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t xml:space="preserve">    57 ( 29.4) </t>
+          <t xml:space="preserve">    47 ( 24.2) </t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t xml:space="preserve">    19 (10.7) </t>
+          <t xml:space="preserve">    29 (16.4) </t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
@@ -3133,120 +3148,223 @@
       </c>
       <c r="H100" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 2.075</t>
+          <t xml:space="preserve"> 0.778</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="B101" t="inlineStr">
         <is>
+          <t>OH+MAFLD</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     9 ( 2.4) </t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     0 (  0.0) </t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     9 ( 5.1) </t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>OH+Virus</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    26 ( 7.0) </t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    20 ( 10.3) </t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     6 ( 3.4) </t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>Virus</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   194 (52.3) </t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   109 ( 56.2) </t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    85 (48.0) </t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>respostHDK_aguda (%)</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    76 (20.5) </t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    57 ( 29.4) </t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    19 (10.7) </t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>&lt;0.001</t>
+        </is>
+      </c>
+      <c r="H104" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 2.075</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="B105" t="inlineStr">
+        <is>
           <t>si</t>
         </is>
       </c>
-      <c r="C101" t="inlineStr">
+      <c r="C105" t="inlineStr">
         <is>
           <t xml:space="preserve">   139 (37.5) </t>
         </is>
       </c>
-      <c r="D101" t="inlineStr">
+      <c r="D105" t="inlineStr">
         <is>
           <t xml:space="preserve">   121 ( 62.4) </t>
         </is>
       </c>
-      <c r="E101" t="inlineStr">
+      <c r="E105" t="inlineStr">
         <is>
           <t xml:space="preserve">    18 (10.2) </t>
         </is>
       </c>
     </row>
-    <row r="102">
-      <c r="C102" t="inlineStr">
+    <row r="106">
+      <c r="C106" t="inlineStr">
         <is>
           <t xml:space="preserve">   156 (42.0) </t>
         </is>
       </c>
-      <c r="D102" t="inlineStr">
+      <c r="D106" t="inlineStr">
         <is>
           <t xml:space="preserve">    16 (  8.2) </t>
         </is>
       </c>
-      <c r="E102" t="inlineStr">
+      <c r="E106" t="inlineStr">
         <is>
           <t xml:space="preserve">   140 (79.1) </t>
         </is>
       </c>
     </row>
-    <row r="103">
-      <c r="A103" t="inlineStr">
+    <row r="107">
+      <c r="A107" t="inlineStr">
         <is>
           <t>respostHDK_crònica (%)</t>
         </is>
       </c>
-      <c r="B103" t="inlineStr">
+      <c r="B107" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="C103" t="inlineStr">
+      <c r="C107" t="inlineStr">
         <is>
           <t xml:space="preserve">    63 (17.0) </t>
         </is>
       </c>
-      <c r="D103" t="inlineStr">
+      <c r="D107" t="inlineStr">
         <is>
           <t xml:space="preserve">    54 ( 27.8) </t>
         </is>
       </c>
-      <c r="E103" t="inlineStr">
+      <c r="E107" t="inlineStr">
         <is>
           <t xml:space="preserve">     9 ( 5.1) </t>
         </is>
       </c>
-      <c r="F103" t="inlineStr">
+      <c r="F107" t="inlineStr">
         <is>
           <t>&lt;0.001</t>
         </is>
       </c>
-      <c r="H103" t="inlineStr">
+      <c r="H107" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1.578</t>
         </is>
       </c>
     </row>
-    <row r="104">
-      <c r="B104" t="inlineStr">
+    <row r="108">
+      <c r="B108" t="inlineStr">
         <is>
           <t>si</t>
         </is>
       </c>
-      <c r="C104" t="inlineStr">
+      <c r="C108" t="inlineStr">
         <is>
           <t xml:space="preserve">    95 (25.6) </t>
         </is>
       </c>
-      <c r="D104" t="inlineStr">
+      <c r="D108" t="inlineStr">
         <is>
           <t xml:space="preserve">    85 ( 43.8) </t>
         </is>
       </c>
-      <c r="E104" t="inlineStr">
+      <c r="E108" t="inlineStr">
         <is>
           <t xml:space="preserve">    10 ( 5.6) </t>
         </is>
       </c>
     </row>
-    <row r="105">
-      <c r="C105" t="inlineStr">
+    <row r="109">
+      <c r="C109" t="inlineStr">
         <is>
           <t xml:space="preserve">   213 (57.4) </t>
         </is>
       </c>
-      <c r="D105" t="inlineStr">
+      <c r="D109" t="inlineStr">
         <is>
           <t xml:space="preserve">    55 ( 28.4) </t>
         </is>
       </c>
-      <c r="E105" t="inlineStr">
+      <c r="E109" t="inlineStr">
         <is>
           <t xml:space="preserve">   158 (89.3) </t>
         </is>

</xml_diff>